<commit_message>
Fixed the insert-rows and column maping
</commit_message>
<xml_diff>
--- a/src/__tests__/services/testAssociatesAndJobs.xlsx
+++ b/src/__tests__/services/testAssociatesAndJobs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18019\OneDrive\Desktop\Sandbox\no-show-software\src\__tests__\services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67741985-1F66-4392-90FC-2C13C92EC74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E96633A-2A54-4EC1-822D-83A8F499ACDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{0434F929-ED76-4B2D-AC70-9DC6C557CDC2}"/>
+    <workbookView xWindow="1820" yWindow="1820" windowWidth="14400" windowHeight="7270" xr2:uid="{0434F929-ED76-4B2D-AC70-9DC6C557CDC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -134,9 +134,6 @@
     <t>Doe</t>
   </si>
   <si>
-    <t>555-1234</t>
-  </si>
-  <si>
     <t>jane.doe@email.com</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t>Smith</t>
   </si>
   <si>
-    <t>555-5678</t>
-  </si>
-  <si>
     <t>john.smith@email.com</t>
   </si>
   <si>
@@ -158,9 +152,6 @@
     <t>Garcia</t>
   </si>
   <si>
-    <t>555-9012</t>
-  </si>
-  <si>
     <t>maria.garcia@email.com</t>
   </si>
   <si>
@@ -170,10 +161,19 @@
     <t>Tanaka</t>
   </si>
   <si>
-    <t>555-3456</t>
-  </si>
-  <si>
     <t>kenji.tanaka@email.com</t>
+  </si>
+  <si>
+    <t>801-555-1234</t>
+  </si>
+  <si>
+    <t>801-555-5678</t>
+  </si>
+  <si>
+    <t>801-555-3456</t>
+  </si>
+  <si>
+    <t>801-555-9012</t>
   </si>
 </sst>
 </file>
@@ -548,21 +548,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830977E1-3116-4733-91EC-04AEA78D4047}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="30.3125" customWidth="1"/>
+    <col min="4" max="4" width="23.7265625" customWidth="1"/>
+    <col min="5" max="5" width="30.26953125" customWidth="1"/>
+    <col min="7" max="7" width="15.6328125" customWidth="1"/>
     <col min="8" max="8" width="32" customWidth="1"/>
-    <col min="9" max="9" width="34.5234375" customWidth="1"/>
-    <col min="10" max="10" width="22.5234375" customWidth="1"/>
-    <col min="11" max="11" width="23.83984375" customWidth="1"/>
-    <col min="12" max="12" width="22.9453125" customWidth="1"/>
+    <col min="9" max="9" width="34.54296875" customWidth="1"/>
+    <col min="10" max="10" width="22.54296875" customWidth="1"/>
+    <col min="11" max="11" width="23.81640625" customWidth="1"/>
+    <col min="12" max="12" width="22.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -597,7 +599,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>101</v>
       </c>
@@ -608,10 +610,10 @@
         <v>31</v>
       </c>
       <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
         <v>32</v>
-      </c>
-      <c r="E2" t="s">
-        <v>33</v>
       </c>
       <c r="F2">
         <v>5001</v>
@@ -638,7 +640,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>101</v>
       </c>
@@ -649,10 +651,10 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
         <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
       </c>
       <c r="F3">
         <v>5002</v>
@@ -679,7 +681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>101</v>
       </c>
@@ -690,10 +692,10 @@
         <v>31</v>
       </c>
       <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
         <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>33</v>
       </c>
       <c r="F4">
         <v>5003</v>
@@ -720,21 +722,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>102</v>
       </c>
       <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
         <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
       </c>
       <c r="F5">
         <v>5004</v>
@@ -761,21 +763,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>103</v>
       </c>
       <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
         <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>41</v>
       </c>
       <c r="F6">
         <v>5005</v>
@@ -802,21 +804,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
         <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>